<commit_message>
remove unused dependencies from conda environment requirements for MacOS
</commit_message>
<xml_diff>
--- a/quize 03-01.xlsx
+++ b/quize 03-01.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chiuw\Dropbox\_Teaching\Northwestern MLDS\Interpretable ML for Finance\IML4Finance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3FDC6BC-5A90-40DE-BD40-131E7E560CA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD07FA8B-237C-4146-9911-D5AD5DBAD5BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="33">
   <si>
     <t>x1</t>
   </si>
@@ -137,6 +137,9 @@
   </si>
   <si>
     <t>Python</t>
+  </si>
+  <si>
+    <t>Term</t>
   </si>
 </sst>
 </file>
@@ -147,7 +150,7 @@
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -168,12 +171,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Consolas"/>
-      <family val="3"/>
     </font>
   </fonts>
   <fills count="6">
@@ -208,7 +205,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -216,12 +213,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
@@ -242,16 +254,25 @@
     <xf numFmtId="3" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -263,20 +284,6 @@
       <fill>
         <patternFill patternType="solid">
           <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="9" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -303,17 +310,7 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0%"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="9" tint="0.79998168889431442"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -327,7 +324,7 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <bgColor theme="5" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -361,6 +358,30 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0%"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -375,7 +396,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Weiliang Chiu" refreshedDate="45752.769080092592" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="19" xr:uid="{99789A65-92F0-4156-92E2-29B23EA5A47C}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="William Chiu" refreshedDate="45752.901501504632" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="19" xr:uid="{99789A65-92F0-4156-92E2-29B23EA5A47C}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:E20" sheet="Data"/>
   </cacheSource>
@@ -552,6 +573,107 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{480B8EE2-DC34-464A-A51C-1741586CE961}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" multipleFieldFilters="0">
+  <location ref="A3:D7" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="5">
+    <pivotField dataField="1" numFmtId="4" showAll="0"/>
+    <pivotField numFmtId="4" showAll="0"/>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="3"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="2"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of x1" fld="0" subtotal="count" baseField="3" baseItem="0" numFmtId="3"/>
+  </dataFields>
+  <formats count="5">
+    <format dxfId="13">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="2" count="0" selected="0"/>
+          <reference field="3" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="12">
+      <pivotArea field="2" grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" axis="axisCol" fieldPosition="0">
+        <references count="1">
+          <reference field="2" count="0" selected="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="11">
+      <pivotArea field="3" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="10">
+      <pivotArea outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="9">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3DAD47D1-96CC-440D-9715-7E9ED6DDD8BE}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" multipleFieldFilters="0">
   <location ref="A10:D14" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
@@ -605,10 +727,10 @@
     <dataField name="Count of x1" fld="0" subtotal="count" showDataAs="percentOfTotal" baseField="3" baseItem="0" numFmtId="164"/>
   </dataFields>
   <formats count="4">
-    <format dxfId="12">
+    <format dxfId="17">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="11">
+    <format dxfId="16">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="2" count="0" selected="0"/>
@@ -616,120 +738,19 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="10">
+    <format dxfId="15">
       <pivotArea field="2" grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" axis="axisCol" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0" selected="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="9">
+    <format dxfId="14">
       <pivotArea field="3" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="3" count="0"/>
         </references>
       </pivotArea>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{480B8EE2-DC34-464A-A51C-1741586CE961}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" multipleFieldFilters="0">
-  <location ref="A3:D7" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="5">
-    <pivotField dataField="1" numFmtId="4" showAll="0"/>
-    <pivotField numFmtId="4" showAll="0"/>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="3"/>
-  </rowFields>
-  <rowItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="2"/>
-  </colFields>
-  <colItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of x1" fld="0" subtotal="count" baseField="3" baseItem="0" numFmtId="3"/>
-  </dataFields>
-  <formats count="5">
-    <format dxfId="17">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="2" count="0" selected="0"/>
-          <reference field="3" count="0"/>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="16">
-      <pivotArea field="2" grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" axis="axisCol" fieldPosition="0">
-        <references count="1">
-          <reference field="2" count="0" selected="0"/>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="15">
-      <pivotArea field="3" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="0"/>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="14">
-      <pivotArea outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="13">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
@@ -798,14 +819,14 @@
     <dataField name="Count of x1" fld="0" subtotal="count" baseField="3" baseItem="0" numFmtId="3"/>
   </dataFields>
   <formats count="5">
-    <format dxfId="6">
+    <format dxfId="4">
       <pivotArea field="2" grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" axis="axisCol" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0" selected="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="5">
+    <format dxfId="3">
       <pivotArea outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -814,17 +835,17 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="4">
+    <format dxfId="2">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="3">
+    <format dxfId="1">
       <pivotArea field="4" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="4" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="1">
+    <format dxfId="0">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="2" count="0" selected="0"/>
@@ -909,14 +930,14 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="2">
+    <format dxfId="6">
       <pivotArea field="4" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="4" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="0">
+    <format dxfId="5">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="2" count="0" selected="0"/>
@@ -1200,405 +1221,405 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="5" width="8.7265625" style="19"/>
+    <col min="1" max="5" width="8.7265625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="19" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="16" t="s">
         <v>4</v>
       </c>
       <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="H1">
-        <f>AVERAGE(A:A)</f>
-        <v>10.584369062234311</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="20">
+      <c r="H1" s="18">
+        <v>10.58</v>
+      </c>
+      <c r="I1" s="18"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="17">
         <v>1.3136060582558393</v>
       </c>
-      <c r="B2" s="20">
+      <c r="B2" s="17">
         <v>0.74674122422740186</v>
       </c>
-      <c r="C2" s="19">
-        <v>0</v>
-      </c>
-      <c r="D2" s="19" t="str">
+      <c r="C2" s="16">
+        <v>0</v>
+      </c>
+      <c r="D2" s="16" t="str">
         <f>IF(A2&lt;$H$1,"x1_bin1","x1_bin2")</f>
         <v>x1_bin1</v>
       </c>
-      <c r="E2" s="19" t="str">
+      <c r="E2" s="16" t="str">
         <f>IF(B2&lt;$H$2,"x2_bin1","x2_bin2")</f>
         <v>x2_bin2</v>
       </c>
       <c r="G2" t="s">
         <v>6</v>
       </c>
-      <c r="H2">
-        <f>AVERAGE(B:B)</f>
-        <v>0.47887506067714591</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="20">
+      <c r="H2" s="18">
+        <v>0.48</v>
+      </c>
+      <c r="I2" s="18"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="17">
         <v>2.884070860101708</v>
       </c>
-      <c r="B3" s="20">
+      <c r="B3" s="17">
         <v>0.17510515710666352</v>
       </c>
-      <c r="C3" s="19">
-        <v>0</v>
-      </c>
-      <c r="D3" s="19" t="str">
+      <c r="C3" s="16">
+        <v>0</v>
+      </c>
+      <c r="D3" s="16" t="str">
         <f>IF(A3&lt;$H$1,"x1_bin1","x1_bin2")</f>
         <v>x1_bin1</v>
       </c>
-      <c r="E3" s="19" t="str">
+      <c r="E3" s="16" t="str">
         <f>IF(B3&lt;$H$2,"x2_bin1","x2_bin2")</f>
         <v>x2_bin1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="20">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" s="17">
         <v>3.7737255479397676</v>
       </c>
-      <c r="B4" s="20">
+      <c r="B4" s="17">
         <v>0.66494542601022366</v>
       </c>
-      <c r="C4" s="19">
-        <v>0</v>
-      </c>
-      <c r="D4" s="19" t="str">
+      <c r="C4" s="16">
+        <v>0</v>
+      </c>
+      <c r="D4" s="16" t="str">
         <f t="shared" ref="D4:D20" si="0">IF(A4&lt;$H$1,"x1_bin1","x1_bin2")</f>
         <v>x1_bin1</v>
       </c>
-      <c r="E4" s="19" t="str">
+      <c r="E4" s="16" t="str">
         <f t="shared" ref="E4:E20" si="1">IF(B4&lt;$H$2,"x2_bin1","x2_bin2")</f>
         <v>x2_bin2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="20">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" s="17">
         <v>4.8844977173548196</v>
       </c>
-      <c r="B5" s="20">
+      <c r="B5" s="17">
         <v>0.37432947148130202</v>
       </c>
-      <c r="C5" s="19">
-        <v>0</v>
-      </c>
-      <c r="D5" s="19" t="str">
+      <c r="C5" s="16">
+        <v>0</v>
+      </c>
+      <c r="D5" s="16" t="str">
         <f t="shared" si="0"/>
         <v>x1_bin1</v>
       </c>
-      <c r="E5" s="19" t="str">
+      <c r="E5" s="16" t="str">
         <f t="shared" si="1"/>
         <v>x2_bin1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="20">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" s="17">
         <v>5.7104552889355675</v>
       </c>
-      <c r="B6" s="20">
+      <c r="B6" s="17">
         <v>0.79991076176428544</v>
       </c>
-      <c r="C6" s="19">
-        <v>0</v>
-      </c>
-      <c r="D6" s="19" t="str">
+      <c r="C6" s="16">
+        <v>0</v>
+      </c>
+      <c r="D6" s="16" t="str">
         <f t="shared" si="0"/>
         <v>x1_bin1</v>
       </c>
-      <c r="E6" s="19" t="str">
+      <c r="E6" s="16" t="str">
         <f t="shared" si="1"/>
         <v>x2_bin2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="20">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="17">
         <v>6.426406992306581</v>
       </c>
-      <c r="B7" s="20">
+      <c r="B7" s="17">
         <v>0.19304659528184176</v>
       </c>
-      <c r="C7" s="19">
-        <v>0</v>
-      </c>
-      <c r="D7" s="19" t="str">
+      <c r="C7" s="16">
+        <v>0</v>
+      </c>
+      <c r="D7" s="16" t="str">
         <f t="shared" si="0"/>
         <v>x1_bin1</v>
       </c>
-      <c r="E7" s="19" t="str">
+      <c r="E7" s="16" t="str">
         <f t="shared" si="1"/>
         <v>x2_bin1</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="20">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" s="17">
         <v>7.5505481434840531</v>
       </c>
-      <c r="B8" s="20">
+      <c r="B8" s="17">
         <v>0.86093557891019168</v>
       </c>
-      <c r="C8" s="19">
-        <v>0</v>
-      </c>
-      <c r="D8" s="19" t="str">
+      <c r="C8" s="16">
+        <v>0</v>
+      </c>
+      <c r="D8" s="16" t="str">
         <f t="shared" si="0"/>
         <v>x1_bin1</v>
       </c>
-      <c r="E8" s="19" t="str">
+      <c r="E8" s="16" t="str">
         <f t="shared" si="1"/>
         <v>x2_bin2</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="20">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" s="17">
         <v>8.7668059648950134</v>
       </c>
-      <c r="B9" s="20">
+      <c r="B9" s="17">
         <v>0.61057698824660522</v>
       </c>
-      <c r="C9" s="19">
-        <v>0</v>
-      </c>
-      <c r="D9" s="19" t="str">
+      <c r="C9" s="16">
+        <v>0</v>
+      </c>
+      <c r="D9" s="16" t="str">
         <f t="shared" si="0"/>
         <v>x1_bin1</v>
       </c>
-      <c r="E9" s="19" t="str">
+      <c r="E9" s="16" t="str">
         <f t="shared" si="1"/>
         <v>x2_bin2</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="20">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" s="17">
         <v>9.3506307568218734</v>
       </c>
-      <c r="B10" s="20">
+      <c r="B10" s="17">
         <v>0.43511544714883765</v>
       </c>
-      <c r="C10" s="19">
-        <v>0</v>
-      </c>
-      <c r="D10" s="19" t="str">
+      <c r="C10" s="16">
+        <v>0</v>
+      </c>
+      <c r="D10" s="16" t="str">
         <f t="shared" si="0"/>
         <v>x1_bin1</v>
       </c>
-      <c r="E10" s="19" t="str">
+      <c r="E10" s="16" t="str">
         <f t="shared" si="1"/>
         <v>x2_bin1</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="20">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" s="17">
         <v>10.471644287602347</v>
       </c>
-      <c r="B11" s="20">
+      <c r="B11" s="17">
         <v>0.16832092301256696</v>
       </c>
-      <c r="C11" s="19">
-        <v>0</v>
-      </c>
-      <c r="D11" s="19" t="str">
+      <c r="C11" s="16">
+        <v>0</v>
+      </c>
+      <c r="D11" s="16" t="str">
         <f t="shared" si="0"/>
         <v>x1_bin1</v>
       </c>
-      <c r="E11" s="19" t="str">
+      <c r="E11" s="16" t="str">
         <f t="shared" si="1"/>
         <v>x2_bin1</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="20">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" s="17">
         <v>11.798047092341735</v>
       </c>
-      <c r="B12" s="20">
+      <c r="B12" s="17">
         <v>0.87404703042578369</v>
       </c>
-      <c r="C12" s="19">
+      <c r="C12" s="16">
         <v>1</v>
       </c>
-      <c r="D12" s="19" t="str">
+      <c r="D12" s="16" t="str">
         <f t="shared" si="0"/>
         <v>x1_bin2</v>
       </c>
-      <c r="E12" s="19" t="str">
+      <c r="E12" s="16" t="str">
         <f t="shared" si="1"/>
         <v>x2_bin2</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="20">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" s="17">
         <v>12.227992963457053</v>
       </c>
-      <c r="B13" s="20">
+      <c r="B13" s="17">
         <v>0.1834825761739961</v>
       </c>
-      <c r="C13" s="19">
+      <c r="C13" s="16">
         <v>1</v>
       </c>
-      <c r="D13" s="19" t="str">
+      <c r="D13" s="16" t="str">
         <f t="shared" si="0"/>
         <v>x1_bin2</v>
       </c>
-      <c r="E13" s="19" t="str">
+      <c r="E13" s="16" t="str">
         <f t="shared" si="1"/>
         <v>x2_bin1</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="20">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14" s="17">
         <v>13.461326495100858</v>
       </c>
-      <c r="B14" s="20">
+      <c r="B14" s="17">
         <v>0.31903415347354624</v>
       </c>
-      <c r="C14" s="19">
+      <c r="C14" s="16">
         <v>1</v>
       </c>
-      <c r="D14" s="19" t="str">
+      <c r="D14" s="16" t="str">
         <f t="shared" si="0"/>
         <v>x1_bin2</v>
       </c>
-      <c r="E14" s="19" t="str">
+      <c r="E14" s="16" t="str">
         <f t="shared" si="1"/>
         <v>x2_bin1</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" s="20">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15" s="17">
         <v>14.435598728914128</v>
       </c>
-      <c r="B15" s="20">
+      <c r="B15" s="17">
         <v>0.55725802010077463</v>
       </c>
-      <c r="C15" s="19">
+      <c r="C15" s="16">
         <v>1</v>
       </c>
-      <c r="D15" s="19" t="str">
+      <c r="D15" s="16" t="str">
         <f t="shared" si="0"/>
         <v>x1_bin2</v>
       </c>
-      <c r="E15" s="19" t="str">
+      <c r="E15" s="16" t="str">
         <f t="shared" si="1"/>
         <v>x2_bin2</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16" s="20">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16" s="17">
         <v>15.79809530699923</v>
       </c>
-      <c r="B16" s="20">
+      <c r="B16" s="17">
         <v>0.72711747706973873</v>
       </c>
-      <c r="C16" s="19">
+      <c r="C16" s="16">
         <v>1</v>
       </c>
-      <c r="D16" s="19" t="str">
+      <c r="D16" s="16" t="str">
         <f t="shared" si="0"/>
         <v>x1_bin2</v>
       </c>
-      <c r="E16" s="19" t="str">
+      <c r="E16" s="16" t="str">
         <f t="shared" si="1"/>
         <v>x2_bin2</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="20">
+      <c r="A17" s="17">
         <v>16.614750321365733</v>
       </c>
-      <c r="B17" s="20">
+      <c r="B17" s="17">
         <v>0.46904934805606047</v>
       </c>
-      <c r="C17" s="19">
+      <c r="C17" s="16">
         <v>1</v>
       </c>
-      <c r="D17" s="19" t="str">
+      <c r="D17" s="16" t="str">
         <f t="shared" si="0"/>
         <v>x1_bin2</v>
       </c>
-      <c r="E17" s="19" t="str">
+      <c r="E17" s="16" t="str">
         <f t="shared" si="1"/>
         <v>x2_bin1</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="20">
+      <c r="A18" s="17">
         <v>17.953038475044565</v>
       </c>
-      <c r="B18" s="20">
+      <c r="B18" s="17">
         <v>3.3033288950706452E-2</v>
       </c>
-      <c r="C18" s="19">
+      <c r="C18" s="16">
         <v>1</v>
       </c>
-      <c r="D18" s="19" t="str">
+      <c r="D18" s="16" t="str">
         <f t="shared" si="0"/>
         <v>x1_bin2</v>
       </c>
-      <c r="E18" s="19" t="str">
+      <c r="E18" s="16" t="str">
         <f t="shared" si="1"/>
         <v>x2_bin1</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="20">
+      <c r="A19" s="17">
         <v>18.095397883891327</v>
       </c>
-      <c r="B19" s="20">
+      <c r="B19" s="17">
         <v>0.39970208010502473</v>
       </c>
-      <c r="C19" s="19">
+      <c r="C19" s="16">
         <v>1</v>
       </c>
-      <c r="D19" s="19" t="str">
+      <c r="D19" s="16" t="str">
         <f t="shared" si="0"/>
         <v>x1_bin2</v>
       </c>
-      <c r="E19" s="19" t="str">
+      <c r="E19" s="16" t="str">
         <f t="shared" si="1"/>
         <v>x2_bin1</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" s="20">
+      <c r="A20" s="17">
         <v>19.586373297639703</v>
       </c>
-      <c r="B20" s="20">
+      <c r="B20" s="17">
         <v>0.50687460532022099</v>
       </c>
-      <c r="C20" s="19">
+      <c r="C20" s="16">
         <v>1</v>
       </c>
-      <c r="D20" s="19" t="str">
+      <c r="D20" s="16" t="str">
         <f t="shared" si="0"/>
         <v>x1_bin2</v>
       </c>
-      <c r="E20" s="19" t="str">
+      <c r="E20" s="16" t="str">
         <f t="shared" si="1"/>
         <v>x2_bin2</v>
       </c>
@@ -1611,10 +1632,583 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F62F419F-ACAD-4DC8-8AC2-C6E767D49198}">
+  <dimension ref="A2:I38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.90625" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="15.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B2" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20" t="str">
+        <f>"y="&amp;B4</f>
+        <v>y=0</v>
+      </c>
+      <c r="H4" s="20" t="str">
+        <f>"y="&amp;C4</f>
+        <v>y=1</v>
+      </c>
+      <c r="I4" s="20" t="str">
+        <f t="shared" ref="I4:I7" si="0">D4</f>
+        <v>Grand Total</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="12">
+        <v>10</v>
+      </c>
+      <c r="C5" s="12"/>
+      <c r="D5" s="13">
+        <v>10</v>
+      </c>
+      <c r="F5" s="20" t="str">
+        <f>A5</f>
+        <v>x1_bin1</v>
+      </c>
+      <c r="G5" s="21">
+        <f>B5</f>
+        <v>10</v>
+      </c>
+      <c r="H5" s="21">
+        <f t="shared" ref="H5:H7" si="1">C5</f>
+        <v>0</v>
+      </c>
+      <c r="I5" s="21">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12">
+        <v>9</v>
+      </c>
+      <c r="D6" s="13">
+        <v>9</v>
+      </c>
+      <c r="F6" s="20" t="str">
+        <f t="shared" ref="F6:F7" si="2">A6</f>
+        <v>x1_bin2</v>
+      </c>
+      <c r="G6" s="21">
+        <f t="shared" ref="G6:G7" si="3">B6</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="21">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="I6" s="21">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="13">
+        <v>10</v>
+      </c>
+      <c r="C7" s="13">
+        <v>9</v>
+      </c>
+      <c r="D7" s="14">
+        <v>19</v>
+      </c>
+      <c r="F7" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>Grand Total</v>
+      </c>
+      <c r="G7" s="21">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="H7" s="21">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="I7" s="21">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B9" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20" t="str">
+        <f>"y="&amp;B11</f>
+        <v>y=0</v>
+      </c>
+      <c r="H11" s="20" t="str">
+        <f>"y="&amp;C11</f>
+        <v>y=1</v>
+      </c>
+      <c r="I11" s="20" t="str">
+        <f t="shared" ref="I11:I14" si="4">D11</f>
+        <v>Grand Total</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="7">
+        <v>0.52631578947368418</v>
+      </c>
+      <c r="C12" s="7">
+        <v>0</v>
+      </c>
+      <c r="D12" s="8">
+        <v>0.52631578947368418</v>
+      </c>
+      <c r="F12" s="20" t="str">
+        <f>A12</f>
+        <v>x1_bin1</v>
+      </c>
+      <c r="G12" s="22">
+        <f>B12</f>
+        <v>0.52631578947368418</v>
+      </c>
+      <c r="H12" s="22">
+        <f t="shared" ref="H12:H14" si="5">C12</f>
+        <v>0</v>
+      </c>
+      <c r="I12" s="22">
+        <f t="shared" si="4"/>
+        <v>0.52631578947368418</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="7">
+        <v>0</v>
+      </c>
+      <c r="C13" s="7">
+        <v>0.47368421052631576</v>
+      </c>
+      <c r="D13" s="8">
+        <v>0.47368421052631576</v>
+      </c>
+      <c r="F13" s="20" t="str">
+        <f t="shared" ref="F13:F14" si="6">A13</f>
+        <v>x1_bin2</v>
+      </c>
+      <c r="G13" s="22">
+        <f t="shared" ref="G13:G14" si="7">B13</f>
+        <v>0</v>
+      </c>
+      <c r="H13" s="22">
+        <f t="shared" si="5"/>
+        <v>0.47368421052631576</v>
+      </c>
+      <c r="I13" s="22">
+        <f t="shared" si="4"/>
+        <v>0.47368421052631576</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="8">
+        <v>0.52631578947368418</v>
+      </c>
+      <c r="C14" s="8">
+        <v>0.47368421052631576</v>
+      </c>
+      <c r="D14" s="4">
+        <v>1</v>
+      </c>
+      <c r="F14" s="20" t="str">
+        <f t="shared" si="6"/>
+        <v>Grand Total</v>
+      </c>
+      <c r="G14" s="22">
+        <f t="shared" si="7"/>
+        <v>0.52631578947368418</v>
+      </c>
+      <c r="H14" s="22">
+        <f t="shared" si="5"/>
+        <v>0.47368421052631576</v>
+      </c>
+      <c r="I14" s="22">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="10">
+        <f>D12</f>
+        <v>0.52631578947368418</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="10">
+        <f>D13</f>
+        <v>0.47368421052631576</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="10">
+        <f>B14</f>
+        <v>0.52631578947368418</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="10">
+        <f>C14</f>
+        <v>0.47368421052631576</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" t="s">
+        <v>24</v>
+      </c>
+      <c r="E23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" s="10">
+        <f>B12</f>
+        <v>0.52631578947368418</v>
+      </c>
+      <c r="C24" s="10">
+        <f>B18*B20</f>
+        <v>0.27700831024930744</v>
+      </c>
+      <c r="D24" s="1">
+        <f>IF(B24=0,0,LN(B24/C24))</f>
+        <v>0.64185388617239481</v>
+      </c>
+      <c r="E24" s="15">
+        <f>B24*D24</f>
+        <v>0.33781783482757621</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25" s="10">
+        <f>C12</f>
+        <v>0</v>
+      </c>
+      <c r="C25" s="10">
+        <f>B18*B21</f>
+        <v>0.24930747922437671</v>
+      </c>
+      <c r="D25" s="1">
+        <f t="shared" ref="D25:D27" si="8">IF(B25=0,0,LN(B25/C25))</f>
+        <v>0</v>
+      </c>
+      <c r="E25" s="15">
+        <f t="shared" ref="E25:E27" si="9">B25*D25</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26" s="10">
+        <f>B13</f>
+        <v>0</v>
+      </c>
+      <c r="C26" s="10">
+        <f>B19*B20</f>
+        <v>0.24930747922437671</v>
+      </c>
+      <c r="D26" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="E26" s="15">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" s="10">
+        <f>C13</f>
+        <v>0.47368421052631576</v>
+      </c>
+      <c r="C27" s="10">
+        <f>B19*B21</f>
+        <v>0.22437673130193903</v>
+      </c>
+      <c r="D27" s="1">
+        <f t="shared" si="8"/>
+        <v>0.74721440183022114</v>
+      </c>
+      <c r="E27" s="15">
+        <f t="shared" si="9"/>
+        <v>0.35394366402484156</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D28" s="1"/>
+      <c r="E28" s="15"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B29" s="4">
+        <f>SUM(B24:B27)</f>
+        <v>1</v>
+      </c>
+      <c r="C29" s="4">
+        <f>SUM(C24:C27)</f>
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="D29" s="1"/>
+      <c r="E29" s="19">
+        <f>SUM(E24:E27)</f>
+        <v>0.69176149885241778</v>
+      </c>
+      <c r="F29" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E30" s="18">
+        <v>0.63982403475437599</v>
+      </c>
+      <c r="F30" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E31" s="18">
+        <f>E29-E30</f>
+        <v>5.1937464098041786E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33" s="4">
+        <f>ROUND(B24,3)</f>
+        <v>0.52600000000000002</v>
+      </c>
+      <c r="C33" s="4">
+        <f t="shared" ref="C33:C36" si="10">ROUND(C24,3)</f>
+        <v>0.27700000000000002</v>
+      </c>
+      <c r="D33">
+        <f>IF(B33=0,0,LN(B33/C33))</f>
+        <v>0.64128370655037126</v>
+      </c>
+      <c r="E33">
+        <f>B33*D33</f>
+        <v>0.33731522964549532</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>20</v>
+      </c>
+      <c r="B34" s="4">
+        <f t="shared" ref="B34:C34" si="11">ROUND(B25,3)</f>
+        <v>0</v>
+      </c>
+      <c r="C34" s="4">
+        <f t="shared" si="10"/>
+        <v>0.249</v>
+      </c>
+      <c r="D34">
+        <f t="shared" ref="D34:D36" si="12">IF(B34=0,0,LN(B34/C34))</f>
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <f t="shared" ref="E34:E36" si="13">B34*D34</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>21</v>
+      </c>
+      <c r="B35" s="4">
+        <f t="shared" ref="B35:C35" si="14">ROUND(B26,3)</f>
+        <v>0</v>
+      </c>
+      <c r="C35" s="4">
+        <f t="shared" si="10"/>
+        <v>0.249</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>22</v>
+      </c>
+      <c r="B36" s="4">
+        <f t="shared" ref="B36:C36" si="15">ROUND(B27,3)</f>
+        <v>0.47399999999999998</v>
+      </c>
+      <c r="C36" s="4">
+        <f t="shared" si="10"/>
+        <v>0.224</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="12"/>
+        <v>0.74956126984003657</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="13"/>
+        <v>0.35529204190417729</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E38" s="18">
+        <f>SUM(E33:E36)</f>
+        <v>0.69260727154967261</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B9:D9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22A7E9B5-27D6-449D-80DC-632AFD3B90DE}">
   <dimension ref="A2:G31"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1629,11 +2223,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
@@ -1659,23 +2253,27 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="B5" s="12">
-        <v>10</v>
-      </c>
-      <c r="C5" s="12"/>
+        <v>5</v>
+      </c>
+      <c r="C5" s="12">
+        <v>5</v>
+      </c>
       <c r="D5" s="13">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="12"/>
+        <v>29</v>
+      </c>
+      <c r="B6" s="12">
+        <v>5</v>
+      </c>
       <c r="C6" s="12">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D6" s="13">
         <v>9</v>
@@ -1703,11 +2301,11 @@
       <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
@@ -1733,13 +2331,13 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="B12" s="7">
-        <v>0.52631578947368418</v>
+        <v>0.26315789473684209</v>
       </c>
       <c r="C12" s="7">
-        <v>0</v>
+        <v>0.26315789473684209</v>
       </c>
       <c r="D12" s="8">
         <v>0.52631578947368418</v>
@@ -1750,13 +2348,13 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="B13" s="7">
-        <v>0</v>
+        <v>0.26315789473684209</v>
       </c>
       <c r="C13" s="7">
-        <v>0.47368421052631576</v>
+        <v>0.21052631578947367</v>
       </c>
       <c r="D13" s="8">
         <v>0.47368421052631576</v>
@@ -1844,7 +2442,7 @@
       </c>
       <c r="B24" s="10">
         <f>B12</f>
-        <v>0.52631578947368418</v>
+        <v>0.26315789473684209</v>
       </c>
       <c r="C24" s="10">
         <f>B18*B20</f>
@@ -1852,11 +2450,11 @@
       </c>
       <c r="D24" s="1">
         <f>IF(B24=0,0,LN(B24/C24))</f>
-        <v>0.64185388617239481</v>
+        <v>-5.129329438755046E-2</v>
       </c>
       <c r="E24" s="15">
         <f>B24*D24</f>
-        <v>0.33781783482757621</v>
+        <v>-1.3498235365144858E-2</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
@@ -1865,7 +2463,7 @@
       </c>
       <c r="B25" s="10">
         <f>C12</f>
-        <v>0</v>
+        <v>0.26315789473684209</v>
       </c>
       <c r="C25" s="10">
         <f>B18*B21</f>
@@ -1873,11 +2471,11 @@
       </c>
       <c r="D25" s="1">
         <f t="shared" ref="D25:D27" si="0">IF(B25=0,0,LN(B25/C25))</f>
-        <v>0</v>
+        <v>5.4067221270275793E-2</v>
       </c>
       <c r="E25" s="15">
         <f t="shared" ref="E25:E27" si="1">B25*D25</f>
-        <v>0</v>
+        <v>1.4228216123756786E-2</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
@@ -1886,7 +2484,7 @@
       </c>
       <c r="B26" s="10">
         <f>B13</f>
-        <v>0</v>
+        <v>0.26315789473684209</v>
       </c>
       <c r="C26" s="10">
         <f>B19*B20</f>
@@ -1894,11 +2492,11 @@
       </c>
       <c r="D26" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5.4067221270275793E-2</v>
       </c>
       <c r="E26" s="15">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.4228216123756786E-2</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
@@ -1907,7 +2505,7 @@
       </c>
       <c r="B27" s="10">
         <f>C13</f>
-        <v>0.47368421052631576</v>
+        <v>0.21052631578947367</v>
       </c>
       <c r="C27" s="10">
         <f>B19*B21</f>
@@ -1915,11 +2513,11 @@
       </c>
       <c r="D27" s="1">
         <f t="shared" si="0"/>
-        <v>0.74721440183022114</v>
+        <v>-6.3715814386107628E-2</v>
       </c>
       <c r="E27" s="15">
         <f t="shared" si="1"/>
-        <v>0.35394366402484156</v>
+        <v>-1.3413855660233185E-2</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
@@ -1927,387 +2525,25 @@
       <c r="E28" s="15"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B29" s="4">
-        <f>SUM(B24:B27)</f>
-        <v>1</v>
-      </c>
-      <c r="C29" s="4">
-        <f>SUM(C24:C27)</f>
-        <v>0.99999999999999989</v>
-      </c>
       <c r="D29" s="1"/>
-      <c r="E29" s="16">
+      <c r="E29" s="19">
         <f>SUM(E24:E27)</f>
-        <v>0.69176149885241778</v>
+        <v>1.5443412221355299E-3</v>
       </c>
       <c r="F29" s="11" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="E30" s="17">
-        <v>0.63982403475437599</v>
+      <c r="E30" s="18">
+        <v>0</v>
       </c>
       <c r="F30" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="E31" s="15">
-        <f>E29-E30</f>
-        <v>5.1937464098041786E-2</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B9:D9"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22A7E9B5-27D6-449D-80DC-632AFD3B90DE}">
-  <dimension ref="A2:G31"/>
-  <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.26953125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B2" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="12">
-        <v>5</v>
-      </c>
-      <c r="C5" s="12">
-        <v>5</v>
-      </c>
-      <c r="D5" s="13">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" s="12">
-        <v>5</v>
-      </c>
-      <c r="C6" s="12">
-        <v>4</v>
-      </c>
-      <c r="D6" s="13">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="13">
-        <v>10</v>
-      </c>
-      <c r="C7" s="13">
-        <v>9</v>
-      </c>
-      <c r="D7" s="14">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B9" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" s="7">
-        <v>0.26315789473684209</v>
-      </c>
-      <c r="C12" s="7">
-        <v>0.26315789473684209</v>
-      </c>
-      <c r="D12" s="8">
-        <v>0.52631578947368418</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="7">
-        <v>0.26315789473684209</v>
-      </c>
-      <c r="C13" s="7">
-        <v>0.21052631578947367</v>
-      </c>
-      <c r="D13" s="8">
-        <v>0.47368421052631576</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="8">
-        <v>0.52631578947368418</v>
-      </c>
-      <c r="C14" s="8">
-        <v>0.47368421052631576</v>
-      </c>
-      <c r="D14" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>15</v>
-      </c>
-      <c r="B18" s="10">
-        <f>D12</f>
-        <v>0.52631578947368418</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>16</v>
-      </c>
-      <c r="B19" s="10">
-        <f>D13</f>
-        <v>0.47368421052631576</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>17</v>
-      </c>
-      <c r="B20" s="10">
-        <f>B14</f>
-        <v>0.52631578947368418</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>18</v>
-      </c>
-      <c r="B21" s="10">
-        <f>C14</f>
-        <v>0.47368421052631576</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B23" t="s">
-        <v>13</v>
-      </c>
-      <c r="C23" t="s">
-        <v>27</v>
-      </c>
-      <c r="D23" t="s">
-        <v>24</v>
-      </c>
-      <c r="E23" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>19</v>
-      </c>
-      <c r="B24" s="10">
-        <f>B12</f>
-        <v>0.26315789473684209</v>
-      </c>
-      <c r="C24" s="10">
-        <f>B18*B20</f>
-        <v>0.27700831024930744</v>
-      </c>
-      <c r="D24" s="1">
-        <f>IF(B24=0,0,LN(B24/C24))</f>
-        <v>-5.129329438755046E-2</v>
-      </c>
-      <c r="E24" s="15">
-        <f>B24*D24</f>
-        <v>-1.3498235365144858E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>20</v>
-      </c>
-      <c r="B25" s="10">
-        <f>C12</f>
-        <v>0.26315789473684209</v>
-      </c>
-      <c r="C25" s="10">
-        <f>B18*B21</f>
-        <v>0.24930747922437671</v>
-      </c>
-      <c r="D25" s="1">
-        <f t="shared" ref="D25:D27" si="0">IF(B25=0,0,LN(B25/C25))</f>
-        <v>5.4067221270275793E-2</v>
-      </c>
-      <c r="E25" s="15">
-        <f t="shared" ref="E25:E27" si="1">B25*D25</f>
-        <v>1.4228216123756786E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>21</v>
-      </c>
-      <c r="B26" s="10">
-        <f>B13</f>
-        <v>0.26315789473684209</v>
-      </c>
-      <c r="C26" s="10">
-        <f>B19*B20</f>
-        <v>0.24930747922437671</v>
-      </c>
-      <c r="D26" s="1">
-        <f t="shared" si="0"/>
-        <v>5.4067221270275793E-2</v>
-      </c>
-      <c r="E26" s="15">
-        <f t="shared" si="1"/>
-        <v>1.4228216123756786E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>22</v>
-      </c>
-      <c r="B27" s="10">
-        <f>C13</f>
-        <v>0.21052631578947367</v>
-      </c>
-      <c r="C27" s="10">
-        <f>B19*B21</f>
-        <v>0.22437673130193903</v>
-      </c>
-      <c r="D27" s="1">
-        <f t="shared" si="0"/>
-        <v>-6.3715814386107628E-2</v>
-      </c>
-      <c r="E27" s="15">
-        <f t="shared" si="1"/>
-        <v>-1.3413855660233185E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="D28" s="1"/>
-      <c r="E28" s="15"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="D29" s="1"/>
-      <c r="E29" s="16">
-        <f>SUM(E24:E27)</f>
-        <v>1.5443412221355299E-3</v>
-      </c>
-      <c r="F29" s="11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="E30">
-        <v>0</v>
-      </c>
-      <c r="F30" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="E31" s="15">
+      <c r="E31" s="18">
         <f>E29-E30</f>
         <v>1.5443412221355299E-3</v>
       </c>

</xml_diff>